<commit_message>
mudanca dos dados de fabrica
</commit_message>
<xml_diff>
--- a/dados/dados_fabrica.xlsx
+++ b/dados/dados_fabrica.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24195" windowHeight="12525"/>
+    <workbookView windowWidth="27795" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,57 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>nivel_automacao</t>
   </si>
   <si>
     <t>operadores</t>
-  </si>
-  <si>
-    <t>104.6</t>
-  </si>
-  <si>
-    <t>99.7</t>
-  </si>
-  <si>
-    <t>95.3</t>
-  </si>
-  <si>
-    <t>95.5</t>
-  </si>
-  <si>
-    <t>85.7</t>
-  </si>
-  <si>
-    <t>72.8</t>
-  </si>
-  <si>
-    <t>79.0</t>
-  </si>
-  <si>
-    <t>70.6</t>
-  </si>
-  <si>
-    <t>66.2</t>
-  </si>
-  <si>
-    <t>63.4</t>
-  </si>
-  <si>
-    <t>59.4</t>
-  </si>
-  <si>
-    <t>60.2</t>
-  </si>
-  <si>
-    <t>52.4</t>
-  </si>
-  <si>
-    <t>44.4</t>
-  </si>
-  <si>
-    <t>34.6</t>
   </si>
 </sst>
 </file>
@@ -75,9 +30,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -111,9 +66,122 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,119 +194,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -249,37 +204,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,25 +360,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,115 +384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,39 +395,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -491,17 +413,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,6 +463,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -540,147 +486,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1051,13 +1006,14 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="26.75" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1072,120 +1028,120 @@
       <c r="A2" s="2">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
+      <c r="B2" s="2">
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
+      <c r="B3" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
+      <c r="B4" s="2">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
+      <c r="B5" s="2">
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>30</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
+      <c r="B6" s="2">
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>35</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
+      <c r="B7" s="2">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>40</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
+      <c r="B8" s="2">
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
         <v>45</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
+      <c r="B9" s="2">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>50</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
+      <c r="B10" s="2">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
         <v>55</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
+      <c r="B11" s="2">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
         <v>60</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
+      <c r="B12" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>65</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
+      <c r="B13" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>70</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>14</v>
+      <c r="B14" s="2">
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
         <v>75</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
+      <c r="B15" s="2">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
         <v>80</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>16</v>
+      <c r="B16" s="2">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>